<commit_message>
Subsection Read in data finished
</commit_message>
<xml_diff>
--- a/data/raw/earnings_data/earnings.xlsx
+++ b/data/raw/earnings_data/earnings.xlsx
@@ -365,28 +365,28 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>age in years</t>
+          <t>age.in.years</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>nationality</t>
+          <t>Nationalität</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>income</t>
+          <t>incEur</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Anna</t>
+          <t>Anna Maria</t>
         </is>
       </c>
       <c r="B2">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -395,7 +395,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2097</t>
+          <t>1689</t>
         </is>
       </c>
     </row>
@@ -407,12 +407,12 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>DE</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>1015</t>
+          <t>875</t>
         </is>
       </c>
     </row>
@@ -423,7 +423,7 @@
         </is>
       </c>
       <c r="B4">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -452,7 +452,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2163</t>
+          <t>2299</t>
         </is>
       </c>
     </row>
@@ -463,7 +463,7 @@
         </is>
       </c>
       <c r="B6">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -472,7 +472,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>1430</t>
+          <t>2522</t>
         </is>
       </c>
     </row>
@@ -483,7 +483,7 @@
         </is>
       </c>
       <c r="B7">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -492,18 +492,18 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>921</t>
+          <t>1060</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Gerda Maria</t>
+          <t>Gerda</t>
         </is>
       </c>
       <c r="B8">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -512,7 +512,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>1437</t>
+          <t>1781</t>
         </is>
       </c>
     </row>
@@ -523,7 +523,7 @@
         </is>
       </c>
       <c r="B9">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -532,7 +532,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2448</t>
+          <t>2463</t>
         </is>
       </c>
     </row>
@@ -543,7 +543,7 @@
         </is>
       </c>
       <c r="B10">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -552,7 +552,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>990</t>
+          <t>1442</t>
         </is>
       </c>
     </row>
@@ -563,7 +563,7 @@
         </is>
       </c>
       <c r="B11">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -572,7 +572,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>1571</t>
+          <t>1404</t>
         </is>
       </c>
     </row>

</xml_diff>